<commit_message>
process stop fixes. local-national imputation
</commit_message>
<xml_diff>
--- a/transit_feed_licenses.xlsx
+++ b/transit_feed_licenses.xlsx
@@ -37,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -51,45 +51,15 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -469,29 +439,81 @@
           <t>msa_id</t>
         </is>
       </c>
-      <c r="B1" s="2" t="n"/>
-      <c r="C1" s="2" t="n"/>
-      <c r="D1" s="2" t="n"/>
-      <c r="E1" s="2" t="n"/>
-      <c r="F1" s="2" t="n"/>
-      <c r="G1" s="2" t="n"/>
-      <c r="H1" s="2" t="n"/>
-      <c r="I1" s="2" t="n"/>
-      <c r="J1" s="2" t="n"/>
-      <c r="K1" s="2" t="n"/>
-      <c r="L1" s="2" t="n"/>
-      <c r="M1" s="2" t="n"/>
-      <c r="N1" s="2" t="n"/>
-      <c r="O1" s="2" t="n"/>
-      <c r="P1" s="2" t="n"/>
-      <c r="Q1" s="2" t="n"/>
-      <c r="R1" s="2" t="n"/>
-      <c r="S1" s="2" t="n"/>
-      <c r="T1" s="2" t="n"/>
-      <c r="U1" s="2" t="n"/>
-      <c r="V1" s="2" t="n"/>
-      <c r="W1" s="2" t="n"/>
-      <c r="X1" s="3" t="n"/>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>city</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>agency_id</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>agency_name</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>agency_url</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>onestop_id</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>attribution_instructions</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>attribution_text</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>commercial_use_allowed</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>create_derived_product</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>redistribution_allowed</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>share_alike_optional</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>spdx_identifier</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>url</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>use_without_attribution</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>static_current</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -43782,7 +43804,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:X1"/>
+    <mergeCell ref="A2:X2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>